<commit_message>
Updated CC Expiration Date
</commit_message>
<xml_diff>
--- a/AdvIVRStoredPM.xlsx
+++ b/AdvIVRStoredPM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF74DA07-C578-4CB9-AE6B-8F27F30FDE19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F248DE-623A-4BF7-8A1F-091A2E310B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="2910" windowWidth="18315" windowHeight="10260" firstSheet="3" activeTab="5" xr2:uid="{85B41B3E-B5F3-4D86-B0EB-E4C43EA08BD6}"/>
+    <workbookView xWindow="4005" yWindow="1575" windowWidth="21585" windowHeight="14940" firstSheet="3" activeTab="4" xr2:uid="{85B41B3E-B5F3-4D86-B0EB-E4C43EA08BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateCCStoredPM" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="271">
   <si>
     <t>CAN</t>
   </si>
@@ -845,6 +845,12 @@
   </si>
   <si>
     <t>1235511178</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>122025</t>
   </si>
 </sst>
 </file>
@@ -6629,9 +6635,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7815927-229B-420D-B556-6514A6C920D3}">
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE2" sqref="AE2:AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6835,13 +6841,13 @@
         <v>154</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>155</v>
+        <v>270</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>157</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -6930,13 +6936,13 @@
         <v>154</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>155</v>
+        <v>270</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>157</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -7025,13 +7031,13 @@
         <v>154</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>155</v>
+        <v>270</v>
       </c>
       <c r="AF4" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>157</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
@@ -7120,13 +7126,13 @@
         <v>154</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>155</v>
+        <v>270</v>
       </c>
       <c r="AF5" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>157</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
@@ -7215,13 +7221,13 @@
         <v>154</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>155</v>
+        <v>270</v>
       </c>
       <c r="AF6" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>157</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
@@ -7310,13 +7316,13 @@
         <v>154</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>155</v>
+        <v>270</v>
       </c>
       <c r="AF7" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>157</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
@@ -7405,13 +7411,13 @@
         <v>154</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>155</v>
+        <v>270</v>
       </c>
       <c r="AF8" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>157</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
@@ -7667,6 +7673,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7675,7 +7682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6024C524-EAFE-41AA-B57C-DE469EA75E7A}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed Card Numbers for FeeData
</commit_message>
<xml_diff>
--- a/AdvIVRStoredPM.xlsx
+++ b/AdvIVRStoredPM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F248DE-623A-4BF7-8A1F-091A2E310B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943A8C6D-5B2F-4DA2-B91F-F471066C8615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="1575" windowWidth="21585" windowHeight="14940" firstSheet="3" activeTab="4" xr2:uid="{85B41B3E-B5F3-4D86-B0EB-E4C43EA08BD6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{85B41B3E-B5F3-4D86-B0EB-E4C43EA08BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateCCStoredPM" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="272">
   <si>
     <t>CAN</t>
   </si>
@@ -851,6 +851,9 @@
   </si>
   <si>
     <t>122025</t>
+  </si>
+  <si>
+    <t>2028</t>
   </si>
 </sst>
 </file>
@@ -907,15 +910,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1233,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F9AEF9-6503-40FE-8219-A319EFB418E3}">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1379,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>24</v>
@@ -1459,7 +1459,7 @@
         <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>24</v>
@@ -1539,7 +1539,7 @@
         <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>24</v>
@@ -1619,7 +1619,7 @@
         <v>22</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>24</v>
@@ -1699,7 +1699,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>24</v>
@@ -1779,7 +1779,7 @@
         <v>22</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>24</v>
@@ -1859,7 +1859,7 @@
         <v>22</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>24</v>
@@ -1927,7 +1927,7 @@
         <v>22</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>24</v>
@@ -1995,7 +1995,7 @@
         <v>22</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>24</v>
@@ -2063,7 +2063,7 @@
         <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>24</v>
@@ -2131,7 +2131,7 @@
         <v>22</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>24</v>
@@ -2211,7 +2211,7 @@
         <v>22</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>24</v>
@@ -2291,7 +2291,7 @@
         <v>22</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>24</v>
@@ -2371,7 +2371,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>24</v>
@@ -2432,6 +2432,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2837,6 +2840,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -4143,6 +4149,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -6628,6 +6637,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -6635,7 +6647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7815927-229B-420D-B556-6514A6C920D3}">
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AE2" sqref="AE2:AE8"/>
     </sheetView>
@@ -6762,7 +6774,7 @@
       <c r="B2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -6857,7 +6869,7 @@
       <c r="B3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -6952,7 +6964,7 @@
       <c r="B4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -7047,7 +7059,7 @@
       <c r="B5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -7142,7 +7154,7 @@
       <c r="B6" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -7237,7 +7249,7 @@
       <c r="B7" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -7332,7 +7344,7 @@
       <c r="B8" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -7427,7 +7439,6 @@
       <c r="B9" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
         <v>133</v>
       </c>
@@ -7463,7 +7474,6 @@
       <c r="B10" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="3"/>
       <c r="D10" s="1" t="s">
         <v>133</v>
       </c>
@@ -7499,7 +7509,6 @@
       <c r="B11" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="3"/>
       <c r="D11" s="1" t="s">
         <v>133</v>
       </c>
@@ -7535,7 +7544,6 @@
       <c r="B12" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="3"/>
       <c r="D12" s="1" t="s">
         <v>133</v>
       </c>
@@ -7571,7 +7579,6 @@
       <c r="B13" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="3"/>
       <c r="D13" s="1" t="s">
         <v>133</v>
       </c>
@@ -7607,7 +7614,6 @@
       <c r="B14" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="3"/>
       <c r="D14" s="1" t="s">
         <v>133</v>
       </c>
@@ -7643,7 +7649,6 @@
       <c r="B15" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="3"/>
       <c r="D15" s="1" t="s">
         <v>133</v>
       </c>
@@ -7675,6 +7680,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -7873,7 +7881,7 @@
       <c r="A3" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>268</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -7922,5 +7930,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated CC Expiration Date in AdvIVRStoredPM Spreadsheet
</commit_message>
<xml_diff>
--- a/AdvIVRStoredPM.xlsx
+++ b/AdvIVRStoredPM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943A8C6D-5B2F-4DA2-B91F-F471066C8615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0A2B1B-4DEF-4C1B-B42B-A33D2CCD179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{85B41B3E-B5F3-4D86-B0EB-E4C43EA08BD6}"/>
+    <workbookView xWindow="-31406" yWindow="1123" windowWidth="28140" windowHeight="11803" activeTab="2" xr2:uid="{85B41B3E-B5F3-4D86-B0EB-E4C43EA08BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateCCStoredPM" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="275">
   <si>
     <t>CAN</t>
   </si>
@@ -854,6 +854,15 @@
   </si>
   <si>
     <t>2028</t>
+  </si>
+  <si>
+    <t>102028</t>
+  </si>
+  <si>
+    <t>Card expiration date is invalid</t>
+  </si>
+  <si>
+    <t>9006</t>
   </si>
 </sst>
 </file>
@@ -935,9 +944,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -975,7 +984,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1081,7 +1090,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1223,7 +1232,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1233,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F9AEF9-6503-40FE-8219-A319EFB418E3}">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1382,7 @@
         <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>22</v>
@@ -1453,7 +1462,7 @@
         <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>22</v>
@@ -1533,7 +1542,7 @@
         <v>34</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>22</v>
@@ -1613,7 +1622,7 @@
         <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>22</v>
@@ -1693,7 +1702,7 @@
         <v>67</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>22</v>
@@ -1773,7 +1782,7 @@
         <v>54</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>22</v>
@@ -1853,7 +1862,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>22</v>
@@ -1921,7 +1930,7 @@
         <v>33</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>22</v>
@@ -1989,7 +1998,7 @@
         <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>22</v>
@@ -2057,7 +2066,7 @@
         <v>35</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>22</v>
@@ -2125,7 +2134,7 @@
         <v>20</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>22</v>
@@ -2205,7 +2214,7 @@
         <v>20</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>22</v>
@@ -2285,7 +2294,7 @@
         <v>20</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>22</v>
@@ -2365,7 +2374,7 @@
         <v>20</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>22</v>
@@ -2443,7 +2452,7 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2582,13 +2591,13 @@
         <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>79</v>
@@ -2650,13 +2659,13 @@
         <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>79</v>
@@ -2718,13 +2727,13 @@
         <v>34</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>79</v>
@@ -2786,13 +2795,13 @@
         <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>79</v>
@@ -2850,9 +2859,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71CA8C4-34F9-4667-883D-8C9AB3ADB60A}">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T23" sqref="T23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,13 +2967,13 @@
         <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>24</v>
@@ -3017,13 +3026,13 @@
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>24</v>
@@ -3076,13 +3085,13 @@
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>24</v>
@@ -3138,13 +3147,13 @@
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>24</v>
@@ -3200,13 +3209,13 @@
         <v>20</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>24</v>
@@ -3259,13 +3268,13 @@
         <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>24</v>
@@ -3318,13 +3327,13 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>24</v>
@@ -3383,7 +3392,7 @@
         <v>22</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>24</v>
@@ -3413,10 +3422,10 @@
         <v>47</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>120</v>
+        <v>274</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>119</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -3439,10 +3448,10 @@
         <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>24</v>
@@ -3498,7 +3507,7 @@
         <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>22</v>
@@ -3557,13 +3566,13 @@
         <v>20</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>25</v>
@@ -3616,13 +3625,13 @@
         <v>20</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>24</v>
@@ -3675,13 +3684,13 @@
         <v>20</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>24</v>
@@ -3734,13 +3743,13 @@
         <v>20</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>24</v>
@@ -3793,13 +3802,13 @@
         <v>20</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>24</v>
@@ -3855,13 +3864,13 @@
         <v>20</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>24</v>
@@ -3917,13 +3926,13 @@
         <v>20</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>24</v>
@@ -3979,13 +3988,13 @@
         <v>106</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>24</v>
@@ -4041,13 +4050,13 @@
         <v>107</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>24</v>
@@ -4103,13 +4112,13 @@
         <v>108</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>24</v>

</xml_diff>